<commit_message>
swapped prior EXP102.pdf form for the new version of the form.
</commit_message>
<xml_diff>
--- a/docassemble/Exp102/data/sources/crime_types.xlsx
+++ b/docassemble/Exp102/data/sources/crime_types.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mylegalaid-my.sharepoint.com/personal/alsauber_mnlegalservices_org/Documents/Suffolk Docassemble/Address Lists/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mylegalaid-my.sharepoint.com/personal/alsauber_mnlegalservices_org/Documents/Suffolk Docassemble/Criminal Expungement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="398" documentId="8_{7785BD83-435A-4B7C-B8F5-E40CD472B2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{414E9073-3878-47F2-ADC1-972497B39A3C}"/>
+  <xr:revisionPtr revIDLastSave="404" documentId="8_{7785BD83-435A-4B7C-B8F5-E40CD472B2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BA26603-8E9E-4035-8C8F-C5A348276418}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{CD4733AD-22F5-40C1-A8D7-2640701DC5B5}"/>
   </bookViews>
@@ -683,9 +683,6 @@
     <t>False Traffic Signal</t>
   </si>
   <si>
-    <t>Crimes Involving Transit; Shotting at Transit Vehicle</t>
-  </si>
-  <si>
     <t>Use of Police Radios During Commission of Crime</t>
   </si>
   <si>
@@ -726,6 +723,9 @@
   </si>
   <si>
     <t>Racketeering</t>
+  </si>
+  <si>
+    <t>Crimes Involving Transit; Shooting at Transit Vehicle</t>
   </si>
 </sst>
 </file>
@@ -1086,8 +1086,8 @@
   <dimension ref="A1:C225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A227" sqref="A227"/>
+      <pane ySplit="1" topLeftCell="A204" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B225" sqref="B225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1110,1459 +1110,1459 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>3</v>
+        <v>168</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>4</v>
+        <v>172</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>5</v>
+        <v>173</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>6</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7">
-        <v>7</v>
+        <v>148</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11">
-        <v>11</v>
+        <v>125</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12">
-        <v>12</v>
+        <v>128</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13">
-        <v>13</v>
+        <v>126</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14">
-        <v>14</v>
+        <v>127</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
         <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
         <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22">
-        <v>21</v>
+        <v>142</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27">
-        <v>26</v>
+        <v>205</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>210</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28">
-        <v>27</v>
+        <v>113</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29">
-        <v>28</v>
+        <v>134</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30">
-        <v>29</v>
+        <v>221</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>225</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31">
-        <v>30</v>
+        <v>150</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33">
-        <v>32</v>
+        <v>162</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35">
-        <v>34</v>
+        <v>213</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="B36" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37">
-        <v>36</v>
+        <v>214</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38">
-        <v>37</v>
+        <v>215</v>
       </c>
       <c r="B38" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39">
-        <v>38</v>
+        <v>216</v>
       </c>
       <c r="B39" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="B40" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41">
-        <v>40</v>
+        <v>181</v>
       </c>
       <c r="B41" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="B42" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+      <c r="C42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="B43" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44">
-        <v>43</v>
+        <v>222</v>
       </c>
       <c r="B44" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45">
-        <v>44</v>
+        <v>151</v>
       </c>
       <c r="B45" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A46">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="B46" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47">
-        <v>46</v>
+        <v>208</v>
       </c>
       <c r="B47" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A48">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="B48" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A49">
-        <v>48</v>
+        <v>178</v>
       </c>
       <c r="B49" t="s">
-        <v>53</v>
+        <v>183</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A50">
-        <v>49</v>
+        <v>210</v>
       </c>
       <c r="B50" t="s">
-        <v>54</v>
+        <v>229</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A51">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="B51" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A52">
-        <v>51</v>
+        <v>191</v>
       </c>
       <c r="B52" t="s">
-        <v>56</v>
+        <v>196</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A53">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="B53" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A54">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="B54" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A55">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B55" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A56">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="B56" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A57">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B57" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A58">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B58" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A59">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B59" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A60">
-        <v>59</v>
+        <v>218</v>
       </c>
       <c r="B60" t="s">
-        <v>64</v>
+        <v>222</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A61">
-        <v>60</v>
+        <v>223</v>
       </c>
       <c r="B61" t="s">
-        <v>65</v>
+        <v>227</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A62">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="B62" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A63">
-        <v>62</v>
+        <v>9</v>
       </c>
       <c r="B63" t="s">
-        <v>67</v>
+        <v>13</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A64">
-        <v>63</v>
+        <v>10</v>
       </c>
       <c r="B64" t="s">
-        <v>68</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A65">
-        <v>64</v>
+        <v>138</v>
       </c>
       <c r="B65" t="s">
-        <v>69</v>
+        <v>143</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A66">
-        <v>65</v>
+        <v>140</v>
       </c>
       <c r="B66" t="s">
-        <v>70</v>
+        <v>145</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A67">
-        <v>66</v>
+        <v>139</v>
       </c>
       <c r="B67" t="s">
-        <v>71</v>
+        <v>144</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A68">
-        <v>67</v>
+        <v>158</v>
       </c>
       <c r="B68" t="s">
-        <v>72</v>
+        <v>163</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A69">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="B69" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A70">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="B70" t="s">
-        <v>74</v>
+        <v>39</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A71">
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="B71" t="s">
-        <v>75</v>
+        <v>110</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A72">
-        <v>71</v>
+        <v>212</v>
       </c>
       <c r="B72" t="s">
-        <v>76</v>
+        <v>216</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A73">
-        <v>72</v>
+        <v>180</v>
       </c>
       <c r="B73" t="s">
-        <v>77</v>
+        <v>185</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A74">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="B74" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A75">
-        <v>74</v>
+        <v>16</v>
       </c>
       <c r="B75" t="s">
-        <v>79</v>
+        <v>20</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A76">
-        <v>75</v>
+        <v>17</v>
       </c>
       <c r="B76" t="s">
-        <v>80</v>
+        <v>22</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A77">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="B77" t="s">
-        <v>81</v>
+        <v>125</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A78">
-        <v>77</v>
+        <v>193</v>
       </c>
       <c r="B78" t="s">
-        <v>82</v>
+        <v>198</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A79">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="B79" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A80">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B80" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A81">
-        <v>80</v>
+        <v>199</v>
       </c>
       <c r="B81" t="s">
-        <v>85</v>
+        <v>204</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A82">
-        <v>81</v>
+        <v>131</v>
       </c>
       <c r="B82" t="s">
-        <v>86</v>
+        <v>136</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A83">
-        <v>82</v>
+        <v>161</v>
       </c>
       <c r="B83" t="s">
-        <v>87</v>
+        <v>166</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A84">
-        <v>83</v>
+        <v>143</v>
       </c>
       <c r="B84" t="s">
-        <v>88</v>
+        <v>148</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A85">
-        <v>84</v>
+        <v>165</v>
       </c>
       <c r="B85" t="s">
-        <v>89</v>
+        <v>170</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A86">
-        <v>85</v>
+        <v>219</v>
       </c>
       <c r="B86" t="s">
-        <v>90</v>
+        <v>223</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A87">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="B87" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A88">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B88" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A89">
-        <v>88</v>
+        <v>28</v>
       </c>
       <c r="B89" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A90">
-        <v>89</v>
+        <v>155</v>
       </c>
       <c r="B90" t="s">
-        <v>94</v>
+        <v>160</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A91">
-        <v>90</v>
+        <v>171</v>
       </c>
       <c r="B91" t="s">
-        <v>95</v>
+        <v>176</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A92">
-        <v>91</v>
+        <v>33</v>
       </c>
       <c r="B92" t="s">
-        <v>96</v>
+        <v>38</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A93">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B93" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A94">
-        <v>93</v>
+        <v>192</v>
       </c>
       <c r="B94" t="s">
-        <v>98</v>
+        <v>197</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A95">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="B95" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A96">
-        <v>95</v>
+        <v>209</v>
       </c>
       <c r="B96" t="s">
-        <v>100</v>
+        <v>214</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A97">
-        <v>96</v>
+        <v>206</v>
       </c>
       <c r="B97" t="s">
-        <v>101</v>
+        <v>211</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A98">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="B98" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A99">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B99" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A100">
-        <v>99</v>
+        <v>17</v>
       </c>
       <c r="B100" t="s">
-        <v>104</v>
+        <v>21</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A101">
-        <v>100</v>
+        <v>26</v>
       </c>
       <c r="B101" t="s">
-        <v>105</v>
+        <v>31</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A102">
-        <v>101</v>
+        <v>203</v>
       </c>
       <c r="B102" t="s">
-        <v>106</v>
+        <v>208</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A103">
-        <v>102</v>
+        <v>160</v>
       </c>
       <c r="B103" t="s">
-        <v>107</v>
+        <v>165</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A104">
-        <v>103</v>
+        <v>135</v>
       </c>
       <c r="B104" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A105">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="B105" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A106">
-        <v>105</v>
+        <v>149</v>
       </c>
       <c r="B106" t="s">
-        <v>110</v>
+        <v>154</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A107">
-        <v>106</v>
+        <v>59</v>
       </c>
       <c r="B107" t="s">
-        <v>111</v>
+        <v>64</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A108">
-        <v>107</v>
+        <v>202</v>
       </c>
       <c r="B108" t="s">
-        <v>112</v>
+        <v>207</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A109">
-        <v>108</v>
+        <v>157</v>
       </c>
       <c r="B109" t="s">
-        <v>113</v>
+        <v>162</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A110">
-        <v>109</v>
+        <v>185</v>
       </c>
       <c r="B110" t="s">
-        <v>114</v>
+        <v>190</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A111">
-        <v>110</v>
+        <v>154</v>
       </c>
       <c r="B111" t="s">
-        <v>115</v>
+        <v>159</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A112">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B112" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A113">
-        <v>112</v>
+        <v>189</v>
       </c>
       <c r="B113" t="s">
-        <v>117</v>
+        <v>194</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A114">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="B114" t="s">
-        <v>118</v>
+        <v>24</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A115">
-        <v>114</v>
+        <v>186</v>
       </c>
       <c r="B115" t="s">
-        <v>119</v>
+        <v>191</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A116">
-        <v>115</v>
+        <v>187</v>
       </c>
       <c r="B116" t="s">
-        <v>120</v>
+        <v>192</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A117">
-        <v>116</v>
+        <v>18</v>
       </c>
       <c r="B117" t="s">
-        <v>121</v>
+        <v>23</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A118">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B118" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A119">
-        <v>118</v>
+        <v>87</v>
       </c>
       <c r="B119" t="s">
-        <v>123</v>
+        <v>92</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A120">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="B120" t="s">
-        <v>124</v>
+        <v>93</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A121">
-        <v>120</v>
+        <v>71</v>
       </c>
       <c r="B121" t="s">
-        <v>125</v>
+        <v>76</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A122">
-        <v>121</v>
+        <v>44</v>
       </c>
       <c r="B122" t="s">
-        <v>126</v>
+        <v>49</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A123">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="B123" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A124">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="B124" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A125">
-        <v>124</v>
+        <v>194</v>
       </c>
       <c r="B125" t="s">
-        <v>129</v>
+        <v>199</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A126">
-        <v>125</v>
+        <v>184</v>
       </c>
       <c r="B126" t="s">
-        <v>130</v>
+        <v>189</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A127">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="B127" t="s">
-        <v>131</v>
+        <v>91</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A128">
-        <v>127</v>
+        <v>197</v>
       </c>
       <c r="B128" t="s">
-        <v>132</v>
+        <v>202</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A129">
-        <v>128</v>
+        <v>198</v>
       </c>
       <c r="B129" t="s">
-        <v>133</v>
+        <v>203</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A130">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B130" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A131">
-        <v>130</v>
+        <v>32</v>
       </c>
       <c r="B131" t="s">
-        <v>135</v>
+        <v>37</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A132">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="B132" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A133">
-        <v>132</v>
+        <v>15</v>
       </c>
       <c r="B133" t="s">
-        <v>137</v>
+        <v>19</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A134">
-        <v>133</v>
+        <v>49</v>
       </c>
       <c r="B134" t="s">
-        <v>138</v>
+        <v>54</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A135">
-        <v>134</v>
+        <v>47</v>
       </c>
       <c r="B135" t="s">
-        <v>139</v>
+        <v>52</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A136">
-        <v>135</v>
+        <v>190</v>
       </c>
       <c r="B136" t="s">
-        <v>140</v>
+        <v>195</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A137">
-        <v>136</v>
+        <v>52</v>
       </c>
       <c r="B137" t="s">
-        <v>141</v>
+        <v>57</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A138">
-        <v>137</v>
+        <v>196</v>
       </c>
       <c r="B138" t="s">
-        <v>142</v>
+        <v>201</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A139">
-        <v>138</v>
+        <v>57</v>
       </c>
       <c r="B139" t="s">
-        <v>143</v>
+        <v>62</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A140">
-        <v>139</v>
+        <v>163</v>
       </c>
       <c r="B140" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A141">
-        <v>140</v>
+        <v>117</v>
       </c>
       <c r="B141" t="s">
-        <v>145</v>
+        <v>122</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A142">
-        <v>141</v>
+        <v>72</v>
       </c>
       <c r="B142" t="s">
-        <v>146</v>
+        <v>77</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A143">
-        <v>142</v>
+        <v>6</v>
       </c>
       <c r="B143" t="s">
-        <v>147</v>
+        <v>10</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A144">
-        <v>143</v>
+        <v>7</v>
       </c>
       <c r="B144" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.45">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A145">
-        <v>144</v>
+        <v>39</v>
       </c>
       <c r="B145" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A146">
-        <v>145</v>
+        <v>40</v>
       </c>
       <c r="B146" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.45">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A147">
-        <v>146</v>
+        <v>85</v>
       </c>
       <c r="B147" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.45">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A148">
-        <v>147</v>
+        <v>110</v>
       </c>
       <c r="B148" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.45">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A149">
-        <v>148</v>
+        <v>200</v>
       </c>
       <c r="B149" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.45">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A150">
-        <v>149</v>
+        <v>79</v>
       </c>
       <c r="B150" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.45">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A151">
-        <v>150</v>
+        <v>207</v>
       </c>
       <c r="B151" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.45">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A152">
-        <v>151</v>
+        <v>21</v>
       </c>
       <c r="B152" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.45">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A153">
-        <v>152</v>
+        <v>22</v>
       </c>
       <c r="B153" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A154">
-        <v>153</v>
+        <v>121</v>
       </c>
       <c r="B154" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.45">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A155">
-        <v>154</v>
+        <v>122</v>
       </c>
       <c r="B155" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.45">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A156">
-        <v>155</v>
+        <v>3</v>
       </c>
       <c r="B156" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="C156" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A157">
-        <v>156</v>
+        <v>4</v>
       </c>
       <c r="B157" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+      <c r="C157" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A158">
-        <v>157</v>
+        <v>5</v>
       </c>
       <c r="B158" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A159">
-        <v>158</v>
+        <v>36</v>
       </c>
       <c r="B159" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.45">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A160">
-        <v>159</v>
+        <v>37</v>
       </c>
       <c r="B160" t="s">
-        <v>164</v>
+        <v>42</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A161">
-        <v>160</v>
+        <v>38</v>
       </c>
       <c r="B161" t="s">
-        <v>165</v>
+        <v>43</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A162">
-        <v>161</v>
+        <v>74</v>
       </c>
       <c r="B162" t="s">
-        <v>166</v>
+        <v>79</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A163">
-        <v>162</v>
+        <v>133</v>
       </c>
       <c r="B163" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A164">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B164" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A165">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="B165" t="s">
-        <v>169</v>
+        <v>200</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A166">
-        <v>165</v>
+        <v>102</v>
       </c>
       <c r="B166" t="s">
-        <v>170</v>
+        <v>107</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A167">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="B167" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A168">
-        <v>167</v>
+        <v>55</v>
       </c>
       <c r="B168" t="s">
-        <v>172</v>
+        <v>60</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A169">
-        <v>168</v>
+        <v>89</v>
       </c>
       <c r="B169" t="s">
-        <v>173</v>
+        <v>94</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A170">
+        <v>164</v>
+      </c>
+      <c r="B170" t="s">
         <v>169</v>
-      </c>
-      <c r="B170" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A171">
-        <v>170</v>
+        <v>83</v>
       </c>
       <c r="B171" t="s">
-        <v>175</v>
+        <v>88</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A172">
-        <v>171</v>
+        <v>183</v>
       </c>
       <c r="B172" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A173">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="B173" t="s">
-        <v>177</v>
+        <v>193</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A174">
-        <v>173</v>
+        <v>137</v>
       </c>
       <c r="B174" t="s">
-        <v>178</v>
+        <v>142</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A175">
-        <v>174</v>
+        <v>136</v>
       </c>
       <c r="B175" t="s">
-        <v>179</v>
+        <v>141</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A176">
-        <v>175</v>
+        <v>112</v>
       </c>
       <c r="B176" t="s">
-        <v>180</v>
+        <v>117</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A177">
-        <v>176</v>
+        <v>116</v>
       </c>
       <c r="B177" t="s">
-        <v>181</v>
+        <v>121</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A178">
-        <v>177</v>
+        <v>114</v>
       </c>
       <c r="B178" t="s">
-        <v>182</v>
+        <v>119</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A179">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B179" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A180">
-        <v>179</v>
+        <v>84</v>
       </c>
       <c r="B180" t="s">
-        <v>184</v>
+        <v>89</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A181">
-        <v>180</v>
+        <v>53</v>
       </c>
       <c r="B181" t="s">
-        <v>185</v>
+        <v>58</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A182">
-        <v>181</v>
+        <v>56</v>
       </c>
       <c r="B182" t="s">
-        <v>186</v>
+        <v>61</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.45">
@@ -2575,343 +2575,343 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A184">
-        <v>183</v>
+        <v>80</v>
       </c>
       <c r="B184" t="s">
-        <v>188</v>
+        <v>85</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A185">
-        <v>184</v>
+        <v>82</v>
       </c>
       <c r="B185" t="s">
-        <v>189</v>
+        <v>87</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A186">
-        <v>185</v>
+        <v>224</v>
       </c>
       <c r="B186" t="s">
-        <v>190</v>
+        <v>228</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A187">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B187" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A188">
-        <v>187</v>
+        <v>118</v>
       </c>
       <c r="B188" t="s">
-        <v>192</v>
+        <v>123</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A189">
-        <v>188</v>
+        <v>153</v>
       </c>
       <c r="B189" t="s">
-        <v>193</v>
+        <v>158</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A190">
-        <v>189</v>
+        <v>92</v>
       </c>
       <c r="B190" t="s">
-        <v>194</v>
+        <v>97</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A191">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="B191" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A192">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="B192" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A193">
-        <v>192</v>
+        <v>123</v>
       </c>
       <c r="B193" t="s">
-        <v>197</v>
+        <v>128</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A194">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="B194" t="s">
-        <v>198</v>
+        <v>175</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A195">
-        <v>194</v>
+        <v>169</v>
       </c>
       <c r="B195" t="s">
-        <v>199</v>
+        <v>174</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A196">
-        <v>195</v>
+        <v>66</v>
       </c>
       <c r="B196" t="s">
-        <v>200</v>
+        <v>71</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A197">
-        <v>196</v>
+        <v>30</v>
       </c>
       <c r="B197" t="s">
-        <v>201</v>
+        <v>35</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A198">
-        <v>197</v>
+        <v>109</v>
       </c>
       <c r="B198" t="s">
-        <v>202</v>
+        <v>114</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A199">
-        <v>198</v>
+        <v>50</v>
       </c>
       <c r="B199" t="s">
-        <v>203</v>
+        <v>55</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A200">
-        <v>199</v>
+        <v>67</v>
       </c>
       <c r="B200" t="s">
-        <v>204</v>
+        <v>72</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A201">
-        <v>200</v>
+        <v>95</v>
       </c>
       <c r="B201" t="s">
-        <v>205</v>
+        <v>100</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A202">
-        <v>201</v>
+        <v>94</v>
       </c>
       <c r="B202" t="s">
-        <v>206</v>
+        <v>99</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A203">
-        <v>202</v>
+        <v>54</v>
       </c>
       <c r="B203" t="s">
-        <v>207</v>
+        <v>59</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A204">
-        <v>203</v>
+        <v>156</v>
       </c>
       <c r="B204" t="s">
-        <v>208</v>
+        <v>161</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A205">
-        <v>204</v>
+        <v>101</v>
       </c>
       <c r="B205" t="s">
-        <v>209</v>
+        <v>106</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A206">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="B206" t="s">
-        <v>210</v>
+        <v>224</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A207">
-        <v>206</v>
+        <v>111</v>
       </c>
       <c r="B207" t="s">
-        <v>211</v>
+        <v>116</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A208">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="B208" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A209">
-        <v>208</v>
+        <v>75</v>
       </c>
       <c r="B209" t="s">
-        <v>213</v>
+        <v>80</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A210">
-        <v>209</v>
+        <v>144</v>
       </c>
       <c r="B210" t="s">
-        <v>214</v>
+        <v>149</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A211">
-        <v>210</v>
+        <v>145</v>
       </c>
       <c r="B211" t="s">
-        <v>215</v>
+        <v>150</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A212">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="B212" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A213">
-        <v>212</v>
+        <v>124</v>
       </c>
       <c r="B213" t="s">
-        <v>217</v>
+        <v>129</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A214">
-        <v>213</v>
+        <v>174</v>
       </c>
       <c r="B214" t="s">
-        <v>218</v>
+        <v>179</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A215">
-        <v>214</v>
+        <v>48</v>
       </c>
       <c r="B215" t="s">
-        <v>219</v>
+        <v>53</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A216">
-        <v>215</v>
+        <v>166</v>
       </c>
       <c r="B216" t="s">
-        <v>220</v>
+        <v>171</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A217">
-        <v>216</v>
+        <v>146</v>
       </c>
       <c r="B217" t="s">
-        <v>221</v>
+        <v>151</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A218">
-        <v>217</v>
+        <v>167</v>
       </c>
       <c r="B218" t="s">
-        <v>222</v>
+        <v>172</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A219">
-        <v>218</v>
+        <v>29</v>
       </c>
       <c r="B219" t="s">
-        <v>223</v>
+        <v>34</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A220">
-        <v>219</v>
+        <v>130</v>
       </c>
       <c r="B220" t="s">
-        <v>224</v>
+        <v>135</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A221">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="B221" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A222">
-        <v>221</v>
+        <v>99</v>
       </c>
       <c r="B222" t="s">
-        <v>226</v>
+        <v>104</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A223">
-        <v>222</v>
+        <v>100</v>
       </c>
       <c r="B223" t="s">
-        <v>227</v>
+        <v>105</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A224">
-        <v>223</v>
+        <v>132</v>
       </c>
       <c r="B224" t="s">
-        <v>228</v>
+        <v>137</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A225">
-        <v>224</v>
+        <v>201</v>
       </c>
       <c r="B225" t="s">
-        <v>229</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B91">
-    <sortCondition ref="A1:A91"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C225">
+    <sortCondition ref="B1:B225"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>